<commit_message>
include Malika's protocol in raw data, My-Table parental care for comparison does not calculate number of visit per sex yet
</commit_message>
<xml_diff>
--- a/R_Compare_tblParentalCare.xlsx
+++ b/R_Compare_tblParentalCare.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="48" windowWidth="13380" windowHeight="8208"/>
+    <workbookView xWindow="11508" yWindow="-12" windowWidth="11544" windowHeight="9132" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="R_Compare_tblParentalCare" sheetId="1" r:id="rId1"/>
+    <sheet name="20160217" sheetId="1" r:id="rId1"/>
+    <sheet name="AndrewsFilewithMalikasProtocol" sheetId="2" r:id="rId2"/>
+    <sheet name="20160322" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3665" uniqueCount="1760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3823" uniqueCount="1863">
   <si>
     <t>DVDRef</t>
   </si>
@@ -5294,6 +5296,315 @@
   </si>
   <si>
     <t>sort</t>
+  </si>
+  <si>
+    <t>2015\VO0047.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0056.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0057.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0058.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0062.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0063.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0067.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0068.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0072.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0075.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0076.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0081.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0085.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0087.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0091.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0092.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0093.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0098.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0105.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0107.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0110.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0111.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0112.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0119.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0120.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0121.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0122.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0123.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0128.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0133.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0136.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0137.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0138.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0140.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0143.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0145.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0146.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0147.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0149.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0150.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0151.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0156.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0157.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0158.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0159.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0163.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0164.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0165.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0166.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0167.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0169.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0170.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0171.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0173.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0174.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0177.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0178.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0179.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0181.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0182.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0184.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0185.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0187.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0189.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0193.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0197.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0198.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0206.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0207.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0209.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0210.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0211.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0214.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0216.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0218.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0220.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0222.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0224.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0225.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0228.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0229.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0230.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0232.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0233.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0237.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0240.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0239.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0243.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0244.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0245.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0247.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0250.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0252.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0254.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0255.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0256.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0257.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0258.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0266.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0268.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0269.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0270.xlsx</t>
+  </si>
+  <si>
+    <t>2015\VO0273.xlsx</t>
   </si>
 </sst>
 </file>
@@ -5437,7 +5748,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5617,6 +5928,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -5778,8 +6101,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6124,9 +6449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1747"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L19" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72667,4 +72992,3751 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J115"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1851</v>
+      </c>
+      <c r="B2">
+        <v>4977</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1858</v>
+      </c>
+      <c r="B3">
+        <v>4987</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>-0.3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1895</v>
+      </c>
+      <c r="B4">
+        <v>5064</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1882</v>
+      </c>
+      <c r="B5">
+        <v>5039</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>-5.6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1793</v>
+      </c>
+      <c r="B6">
+        <v>4823</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>-0.1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1789</v>
+      </c>
+      <c r="B7">
+        <v>4805</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1867</v>
+      </c>
+      <c r="B8">
+        <v>5012</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>-0.9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1902</v>
+      </c>
+      <c r="B9">
+        <v>5078</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>-0.2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1856</v>
+      </c>
+      <c r="B10">
+        <v>4984</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>-1.7</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1896</v>
+      </c>
+      <c r="B11">
+        <v>5065</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>-0.1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1899</v>
+      </c>
+      <c r="B12">
+        <v>5073</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1841</v>
+      </c>
+      <c r="B13">
+        <v>4963</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1829</v>
+      </c>
+      <c r="B14">
+        <v>4940</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1885</v>
+      </c>
+      <c r="B15">
+        <v>5044</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>-4.2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1860</v>
+      </c>
+      <c r="B16">
+        <v>4990</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>-1.4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1859</v>
+      </c>
+      <c r="B17">
+        <v>4988</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1854</v>
+      </c>
+      <c r="B18">
+        <v>4980</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>-0.9</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1833</v>
+      </c>
+      <c r="B19">
+        <v>4946</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1857</v>
+      </c>
+      <c r="B20">
+        <v>4986</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1897</v>
+      </c>
+      <c r="B21">
+        <v>5066</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J21" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1868</v>
+      </c>
+      <c r="B22">
+        <v>5013</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="J22" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1871</v>
+      </c>
+      <c r="B23">
+        <v>5019</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>-0.6</v>
+      </c>
+      <c r="J23" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1877</v>
+      </c>
+      <c r="B24">
+        <v>5031</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J24" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1881</v>
+      </c>
+      <c r="B25">
+        <v>5037</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1873</v>
+      </c>
+      <c r="B26">
+        <v>5023</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="J26" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1849</v>
+      </c>
+      <c r="B27">
+        <v>4974</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>-4.3</v>
+      </c>
+      <c r="J27" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1875</v>
+      </c>
+      <c r="B28">
+        <v>5027</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>-4.3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1850</v>
+      </c>
+      <c r="B29">
+        <v>4976</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>-4</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1803</v>
+      </c>
+      <c r="B30">
+        <v>4862</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>-3.8</v>
+      </c>
+      <c r="J30" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1837</v>
+      </c>
+      <c r="B31">
+        <v>4954</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>-3.6</v>
+      </c>
+      <c r="J31" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1893</v>
+      </c>
+      <c r="B32">
+        <v>5062</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>-3.3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>1901</v>
+      </c>
+      <c r="B33">
+        <v>5075</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>-3.3</v>
+      </c>
+      <c r="J33" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>1804</v>
+      </c>
+      <c r="B34">
+        <v>4866</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>-3.2</v>
+      </c>
+      <c r="J34" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1824</v>
+      </c>
+      <c r="B35">
+        <v>4925</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>-2.5</v>
+      </c>
+      <c r="J35" t="s">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1844</v>
+      </c>
+      <c r="B36">
+        <v>4966</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>-2.5</v>
+      </c>
+      <c r="J36" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1808</v>
+      </c>
+      <c r="B37">
+        <v>4876</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="J37" t="s">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1812</v>
+      </c>
+      <c r="B38">
+        <v>4889</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="J38" t="s">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1821</v>
+      </c>
+      <c r="B39">
+        <v>4916</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>-2.1</v>
+      </c>
+      <c r="J39" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1845</v>
+      </c>
+      <c r="B40">
+        <v>4968</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>-2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1830</v>
+      </c>
+      <c r="B41">
+        <v>4943</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>-1.8</v>
+      </c>
+      <c r="J41" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>1807</v>
+      </c>
+      <c r="B42">
+        <v>4872</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>-1.7</v>
+      </c>
+      <c r="J42" t="s">
+        <v>1767</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1865</v>
+      </c>
+      <c r="B43">
+        <v>5003</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>-1.7</v>
+      </c>
+      <c r="J43" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>1823</v>
+      </c>
+      <c r="B44">
+        <v>4924</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>-1.6</v>
+      </c>
+      <c r="J44" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>1838</v>
+      </c>
+      <c r="B45">
+        <v>4955</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>-1.6</v>
+      </c>
+      <c r="J45" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>1855</v>
+      </c>
+      <c r="B46">
+        <v>4983</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>-1.6</v>
+      </c>
+      <c r="J46" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>1843</v>
+      </c>
+      <c r="B47">
+        <v>4965</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>-1.5</v>
+      </c>
+      <c r="J47" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>1790</v>
+      </c>
+      <c r="B48">
+        <v>4806</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>-1.2</v>
+      </c>
+      <c r="J48" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1847</v>
+      </c>
+      <c r="B49">
+        <v>4972</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>-1.2</v>
+      </c>
+      <c r="J49" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>1853</v>
+      </c>
+      <c r="B50">
+        <v>4979</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>-1.2</v>
+      </c>
+      <c r="J50" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1835</v>
+      </c>
+      <c r="B51">
+        <v>4951</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="J51" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>1839</v>
+      </c>
+      <c r="B52">
+        <v>4956</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="J52" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>1879</v>
+      </c>
+      <c r="B53">
+        <v>5035</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="J53" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1797</v>
+      </c>
+      <c r="B54">
+        <v>4845</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>-1</v>
+      </c>
+      <c r="J54" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1840</v>
+      </c>
+      <c r="B55">
+        <v>4957</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>-0.9</v>
+      </c>
+      <c r="J55" t="s">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>1846</v>
+      </c>
+      <c r="B56">
+        <v>4971</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>-0.9</v>
+      </c>
+      <c r="J56" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>1794</v>
+      </c>
+      <c r="B57">
+        <v>4835</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>-0.8</v>
+      </c>
+      <c r="J57" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>1796</v>
+      </c>
+      <c r="B58">
+        <v>4842</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>-0.8</v>
+      </c>
+      <c r="J58" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>1852</v>
+      </c>
+      <c r="B59">
+        <v>4978</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>-0.8</v>
+      </c>
+      <c r="J59" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>1880</v>
+      </c>
+      <c r="B60">
+        <v>5036</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>-0.8</v>
+      </c>
+      <c r="J60" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>1799</v>
+      </c>
+      <c r="B61">
+        <v>4847</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>-0.7</v>
+      </c>
+      <c r="J61" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>1814</v>
+      </c>
+      <c r="B62">
+        <v>4891</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>-0.6</v>
+      </c>
+      <c r="J62" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>1826</v>
+      </c>
+      <c r="B63">
+        <v>4927</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>-0.6</v>
+      </c>
+      <c r="J63" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>1874</v>
+      </c>
+      <c r="B64">
+        <v>5026</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>-0.6</v>
+      </c>
+      <c r="J64" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>1870</v>
+      </c>
+      <c r="B65">
+        <v>5018</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>-0.5</v>
+      </c>
+      <c r="J65" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>1876</v>
+      </c>
+      <c r="B66">
+        <v>5030</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>-0.5</v>
+      </c>
+      <c r="J66" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>1898</v>
+      </c>
+      <c r="B67">
+        <v>5070</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>-0.5</v>
+      </c>
+      <c r="J67" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>1798</v>
+      </c>
+      <c r="B68">
+        <v>4846</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>-0.4</v>
+      </c>
+      <c r="J68" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>1801</v>
+      </c>
+      <c r="B69">
+        <v>4860</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>-0.4</v>
+      </c>
+      <c r="J69" t="s">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>1805</v>
+      </c>
+      <c r="B70">
+        <v>4867</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>-0.4</v>
+      </c>
+      <c r="J70" t="s">
+        <v>1765</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>1825</v>
+      </c>
+      <c r="B71">
+        <v>4926</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>-0.4</v>
+      </c>
+      <c r="J71" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>1848</v>
+      </c>
+      <c r="B72">
+        <v>4973</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>-0.4</v>
+      </c>
+      <c r="J72" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>1890</v>
+      </c>
+      <c r="B73">
+        <v>5055</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>-0.4</v>
+      </c>
+      <c r="J73" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>1795</v>
+      </c>
+      <c r="B74">
+        <v>4836</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>-0.3</v>
+      </c>
+      <c r="J74" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>1842</v>
+      </c>
+      <c r="B75">
+        <v>4964</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>-0.2</v>
+      </c>
+      <c r="J75" t="s">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>1866</v>
+      </c>
+      <c r="B76">
+        <v>5006</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>-0.2</v>
+      </c>
+      <c r="J76" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>1869</v>
+      </c>
+      <c r="B77">
+        <v>5017</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>-0.2</v>
+      </c>
+      <c r="J77" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>1891</v>
+      </c>
+      <c r="B78">
+        <v>5058</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>-0.2</v>
+      </c>
+      <c r="J78" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>1894</v>
+      </c>
+      <c r="B79">
+        <v>5063</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>-0.2</v>
+      </c>
+      <c r="J79" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>1809</v>
+      </c>
+      <c r="B80">
+        <v>4879</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>-0.1</v>
+      </c>
+      <c r="J80" t="s">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>1813</v>
+      </c>
+      <c r="B81">
+        <v>4890</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>-0.1</v>
+      </c>
+      <c r="J81" t="s">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>1886</v>
+      </c>
+      <c r="B82">
+        <v>5050</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>-0.1</v>
+      </c>
+      <c r="J82" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>1888</v>
+      </c>
+      <c r="B83">
+        <v>5052</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>-0.1</v>
+      </c>
+      <c r="J83" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>1889</v>
+      </c>
+      <c r="B84">
+        <v>5053</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>-0.1</v>
+      </c>
+      <c r="J84" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>1791</v>
+      </c>
+      <c r="B85">
+        <v>4816</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>1792</v>
+      </c>
+      <c r="B86">
+        <v>4818</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>1800</v>
+      </c>
+      <c r="B87">
+        <v>4852</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>1802</v>
+      </c>
+      <c r="B88">
+        <v>4861</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>1810</v>
+      </c>
+      <c r="B89">
+        <v>4880</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>1822</v>
+      </c>
+      <c r="B90">
+        <v>4917</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>1806</v>
+      </c>
+      <c r="B91">
+        <v>4871</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J91" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>1811</v>
+      </c>
+      <c r="B92">
+        <v>4883</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J92" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>1815</v>
+      </c>
+      <c r="B93">
+        <v>4897</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J93" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>1816</v>
+      </c>
+      <c r="B94">
+        <v>4898</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J94" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>1817</v>
+      </c>
+      <c r="B95">
+        <v>4903</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J95" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>1818</v>
+      </c>
+      <c r="B96">
+        <v>4910</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J96" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>1819</v>
+      </c>
+      <c r="B97">
+        <v>4911</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J97" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>1820</v>
+      </c>
+      <c r="B98">
+        <v>4915</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J98" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>1827</v>
+      </c>
+      <c r="B99">
+        <v>4928</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J99" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>1828</v>
+      </c>
+      <c r="B100">
+        <v>4934</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J100" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>1831</v>
+      </c>
+      <c r="B101">
+        <v>4944</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J101" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>1832</v>
+      </c>
+      <c r="B102">
+        <v>4945</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J102" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>1834</v>
+      </c>
+      <c r="B103">
+        <v>4949</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J103" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>1836</v>
+      </c>
+      <c r="B104">
+        <v>4953</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J104" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>1861</v>
+      </c>
+      <c r="B105">
+        <v>4991</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J105" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>1862</v>
+      </c>
+      <c r="B106">
+        <v>4993</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J106" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>1863</v>
+      </c>
+      <c r="B107">
+        <v>4995</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J107" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>1864</v>
+      </c>
+      <c r="B108">
+        <v>5001</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J108" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>1872</v>
+      </c>
+      <c r="B109">
+        <v>5022</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J109" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>1878</v>
+      </c>
+      <c r="B110">
+        <v>5032</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J110" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>1883</v>
+      </c>
+      <c r="B111">
+        <v>5040</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J111" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>1884</v>
+      </c>
+      <c r="B112">
+        <v>5043</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J112" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>1887</v>
+      </c>
+      <c r="B113">
+        <v>5051</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J113" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>1892</v>
+      </c>
+      <c r="B114">
+        <v>5060</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J114" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>1900</v>
+      </c>
+      <c r="B115">
+        <v>5074</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J115" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:K115">
+    <sortCondition descending="1" ref="H2"/>
+  </sortState>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>